<commit_message>
Refactoring & includes plans from Communes Peu Peuplées
</commit_message>
<xml_diff>
--- a/bin/data/T_11_06_2_10_cppfix.xlsx
+++ b/bin/data/T_11_06_2_10_cppfix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Files\Uni\Projet Bachelor\Population Generation\Git\node-matsim-population-generator\bin\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B1A395B5-8FDF-4839-80A8-3FB401295F47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AAD784A-DA93-411E-AFED-FF41FBC1667D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="138">
   <si>
     <t>Total</t>
   </si>
@@ -166,20 +166,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Autres communes… </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="8"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>(6)</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">de 2013 à 2017 </t>
     </r>
     <r>
@@ -492,7 +478,7 @@
     <numFmt numFmtId="164" formatCode="00&quot; - &quot;00"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="8"/>
       <color theme="1"/>
@@ -548,19 +534,6 @@
     <font>
       <sz val="8"/>
       <color indexed="8"/>
-      <name val="Arial Narrow"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="8"/>
-      <name val="Arial Narrow"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="8"/>
       <name val="Arial Narrow"/>
       <family val="2"/>
     </font>
@@ -659,7 +632,7 @@
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="left"/>
     </xf>
@@ -675,18 +648,18 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -697,20 +670,20 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -726,10 +699,12 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1154,8 +1129,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BE48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -1290,11 +1265,11 @@
     </row>
     <row r="4" spans="1:57" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AD4" s="24"/>
       <c r="BE4" s="24" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:57" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -1661,24 +1636,24 @@
       </c>
       <c r="D14" s="22"/>
       <c r="E14" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F14" s="23">
         <v>72.7</v>
       </c>
       <c r="G14" s="22"/>
       <c r="H14" s="21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I14" s="23">
         <v>77.8</v>
       </c>
       <c r="J14" s="22"/>
       <c r="K14" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="L14" s="22" t="s">
         <v>42</v>
-      </c>
-      <c r="L14" s="22" t="s">
-        <v>43</v>
       </c>
       <c r="M14" s="22"/>
       <c r="N14" s="21">
@@ -1689,91 +1664,91 @@
       </c>
       <c r="P14" s="22"/>
       <c r="Q14" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="R14" s="22" t="s">
         <v>42</v>
-      </c>
-      <c r="R14" s="22" t="s">
-        <v>43</v>
       </c>
       <c r="S14" s="22"/>
       <c r="T14" s="21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="U14" s="22">
         <v>36.799999999999997</v>
       </c>
       <c r="V14" s="22"/>
       <c r="W14" s="21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="X14" s="23">
         <v>63.8</v>
       </c>
       <c r="Y14" s="22"/>
       <c r="Z14" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AA14" s="22">
         <v>40.700000000000003</v>
       </c>
       <c r="AB14" s="22"/>
       <c r="AC14" s="21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AD14" s="22">
         <v>57.5</v>
       </c>
       <c r="AE14" s="22"/>
       <c r="AF14" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG14" s="22" t="s">
         <v>42</v>
-      </c>
-      <c r="AG14" s="22" t="s">
-        <v>43</v>
       </c>
       <c r="AH14" s="22"/>
       <c r="AI14" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AJ14" s="22">
         <v>40.700000000000003</v>
       </c>
       <c r="AK14" s="22"/>
       <c r="AL14" s="21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AM14" s="22">
         <v>63.7</v>
       </c>
       <c r="AN14" s="22"/>
       <c r="AO14" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="AP14" s="22" t="s">
         <v>42</v>
-      </c>
-      <c r="AP14" s="22" t="s">
-        <v>43</v>
       </c>
       <c r="AQ14" s="22"/>
       <c r="AR14" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="AS14" s="22" t="s">
         <v>42</v>
-      </c>
-      <c r="AS14" s="22" t="s">
-        <v>43</v>
       </c>
       <c r="AT14" s="22"/>
       <c r="AU14" s="21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AV14" s="23">
         <v>31.4</v>
       </c>
       <c r="AW14" s="22"/>
       <c r="AX14" s="21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AY14" s="22">
         <v>39.799999999999997</v>
       </c>
       <c r="AZ14" s="22"/>
       <c r="BA14" s="21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="BB14" s="22">
         <v>67.599999999999994</v>
@@ -1889,7 +1864,7 @@
       </c>
       <c r="AQ15" s="22"/>
       <c r="AR15" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AS15" s="22">
         <v>28.8</v>
@@ -1928,14 +1903,14 @@
         <v>13</v>
       </c>
       <c r="B16" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="22" t="s">
         <v>42</v>
-      </c>
-      <c r="C16" s="22" t="s">
-        <v>43</v>
       </c>
       <c r="D16" s="22"/>
       <c r="E16" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F16" s="23">
         <v>39.299999999999997</v>
@@ -1949,7 +1924,7 @@
       </c>
       <c r="J16" s="22"/>
       <c r="K16" s="21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L16" s="23">
         <v>32.299999999999997</v>
@@ -1963,35 +1938,35 @@
       </c>
       <c r="P16" s="22"/>
       <c r="Q16" s="21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="R16" s="23">
         <v>86</v>
       </c>
       <c r="S16" s="22"/>
       <c r="T16" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="U16" s="23">
         <v>33.200000000000003</v>
       </c>
       <c r="V16" s="22"/>
       <c r="W16" s="21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="X16" s="23">
         <v>55.1</v>
       </c>
       <c r="Y16" s="22"/>
       <c r="Z16" s="21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AA16" s="23">
         <v>45.1</v>
       </c>
       <c r="AB16" s="22"/>
       <c r="AC16" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AD16" s="23">
         <v>60.4</v>
@@ -2005,42 +1980,42 @@
       </c>
       <c r="AH16" s="22"/>
       <c r="AI16" s="21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AJ16" s="23">
         <v>40</v>
       </c>
       <c r="AK16" s="22"/>
       <c r="AL16" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AM16" s="23">
         <v>78.099999999999994</v>
       </c>
       <c r="AN16" s="22"/>
       <c r="AO16" s="21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AP16" s="23">
         <v>45</v>
       </c>
       <c r="AQ16" s="22"/>
       <c r="AR16" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AS16" s="23">
         <v>72.3</v>
       </c>
       <c r="AT16" s="22"/>
       <c r="AU16" s="21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AV16" s="23">
         <v>58.3</v>
       </c>
       <c r="AW16" s="22"/>
       <c r="AX16" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AY16" s="23">
         <v>67.8</v>
@@ -2065,21 +2040,21 @@
         <v>14</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C17" s="23">
         <v>78.099999999999994</v>
       </c>
       <c r="D17" s="22"/>
       <c r="E17" s="21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F17" s="23">
         <v>49.1</v>
       </c>
       <c r="G17" s="22"/>
       <c r="H17" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I17" s="23">
         <v>46.4</v>
@@ -2100,91 +2075,91 @@
       </c>
       <c r="P17" s="22"/>
       <c r="Q17" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="R17" s="22" t="s">
         <v>42</v>
-      </c>
-      <c r="R17" s="22" t="s">
-        <v>43</v>
       </c>
       <c r="S17" s="22"/>
       <c r="T17" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="U17" s="23">
         <v>39</v>
       </c>
       <c r="V17" s="22"/>
       <c r="W17" s="21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="X17" s="22">
         <v>67.5</v>
       </c>
       <c r="Y17" s="22"/>
       <c r="Z17" s="21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AA17" s="22">
         <v>57.6</v>
       </c>
       <c r="AB17" s="22"/>
       <c r="AC17" s="21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AD17" s="22">
         <v>55.1</v>
       </c>
       <c r="AE17" s="22"/>
       <c r="AF17" s="21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AG17" s="22">
         <v>27.3</v>
       </c>
       <c r="AH17" s="22"/>
       <c r="AI17" s="21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AJ17" s="22">
         <v>43.7</v>
       </c>
       <c r="AK17" s="22"/>
       <c r="AL17" s="21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AM17" s="22">
         <v>63.7</v>
       </c>
       <c r="AN17" s="22"/>
       <c r="AO17" s="21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AP17" s="23">
         <v>64</v>
       </c>
       <c r="AQ17" s="22"/>
       <c r="AR17" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="AS17" s="22" t="s">
         <v>42</v>
-      </c>
-      <c r="AS17" s="22" t="s">
-        <v>43</v>
       </c>
       <c r="AT17" s="22"/>
       <c r="AU17" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="AV17" s="22" t="s">
         <v>42</v>
-      </c>
-      <c r="AV17" s="22" t="s">
-        <v>43</v>
       </c>
       <c r="AW17" s="22"/>
       <c r="AX17" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AY17" s="22">
         <v>72.3</v>
       </c>
       <c r="AZ17" s="22"/>
       <c r="BA17" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="BB17" s="22">
         <v>29.9</v>
@@ -2339,28 +2314,28 @@
         <v>16</v>
       </c>
       <c r="B19" s="21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C19" s="22">
         <v>35.5</v>
       </c>
       <c r="D19" s="22"/>
       <c r="E19" s="21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F19" s="22">
         <v>28.3</v>
       </c>
       <c r="G19" s="22"/>
       <c r="H19" s="21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I19" s="23">
         <v>53.1</v>
       </c>
       <c r="J19" s="22"/>
       <c r="K19" s="21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L19" s="22">
         <v>51.6</v>
@@ -2395,21 +2370,21 @@
       </c>
       <c r="Y19" s="22"/>
       <c r="Z19" s="21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AA19" s="22">
         <v>33.9</v>
       </c>
       <c r="AB19" s="22"/>
       <c r="AC19" s="21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AD19" s="23">
         <v>44</v>
       </c>
       <c r="AE19" s="22"/>
       <c r="AF19" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AG19" s="22">
         <v>41.7</v>
@@ -2423,21 +2398,21 @@
       </c>
       <c r="AK19" s="22"/>
       <c r="AL19" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AM19" s="23">
         <v>28.7</v>
       </c>
       <c r="AN19" s="22"/>
       <c r="AO19" s="21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AP19" s="22">
         <v>41</v>
       </c>
       <c r="AQ19" s="22"/>
       <c r="AR19" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AS19" s="22">
         <v>29.5</v>
@@ -2451,14 +2426,14 @@
       </c>
       <c r="AW19" s="22"/>
       <c r="AX19" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AY19" s="22">
         <v>37.5</v>
       </c>
       <c r="AZ19" s="22"/>
       <c r="BA19" s="21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="BB19" s="22">
         <v>32.9</v>
@@ -2490,14 +2465,14 @@
       </c>
       <c r="G20" s="22"/>
       <c r="H20" s="21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I20" s="23">
         <v>35</v>
       </c>
       <c r="J20" s="22"/>
       <c r="K20" s="21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L20" s="23">
         <v>39.1</v>
@@ -2574,7 +2549,7 @@
       </c>
       <c r="AQ20" s="22"/>
       <c r="AR20" s="21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AS20" s="23">
         <v>28.2</v>
@@ -2627,14 +2602,14 @@
       </c>
       <c r="G21" s="22"/>
       <c r="H21" s="21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I21" s="23">
         <v>45.4</v>
       </c>
       <c r="J21" s="22"/>
       <c r="K21" s="21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L21" s="22">
         <v>36.9</v>
@@ -2676,14 +2651,14 @@
       </c>
       <c r="AB21" s="22"/>
       <c r="AC21" s="21" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AD21" s="22">
         <v>31.1</v>
       </c>
       <c r="AE21" s="22"/>
       <c r="AF21" s="21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AG21" s="22">
         <v>33.4</v>
@@ -2704,7 +2679,7 @@
       </c>
       <c r="AN21" s="22"/>
       <c r="AO21" s="21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AP21" s="23">
         <v>35</v>
@@ -2750,28 +2725,28 @@
         <v>19</v>
       </c>
       <c r="B22" s="21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C22" s="22">
         <v>34.9</v>
       </c>
       <c r="D22" s="22"/>
       <c r="E22" s="21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F22" s="22">
         <v>30.5</v>
       </c>
       <c r="G22" s="22"/>
       <c r="H22" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="I22" s="22" t="s">
         <v>42</v>
-      </c>
-      <c r="I22" s="22" t="s">
-        <v>43</v>
       </c>
       <c r="J22" s="22"/>
       <c r="K22" s="22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L22" s="22">
         <v>60.3</v>
@@ -2785,7 +2760,7 @@
       </c>
       <c r="P22" s="22"/>
       <c r="Q22" s="22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="R22" s="22">
         <v>60.3</v>
@@ -2799,7 +2774,7 @@
       </c>
       <c r="V22" s="22"/>
       <c r="W22" s="22" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="X22" s="23">
         <v>44</v>
@@ -2813,63 +2788,63 @@
       </c>
       <c r="AB22" s="22"/>
       <c r="AC22" s="22" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AD22" s="22">
         <v>48.1</v>
       </c>
       <c r="AE22" s="22"/>
       <c r="AF22" s="22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AG22" s="22">
         <v>55.1</v>
       </c>
       <c r="AH22" s="22"/>
       <c r="AI22" s="22" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AJ22" s="23">
         <v>28.7</v>
       </c>
       <c r="AK22" s="22"/>
       <c r="AL22" s="22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AM22" s="23">
         <v>51.3</v>
       </c>
       <c r="AN22" s="22"/>
       <c r="AO22" s="22" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AP22" s="22">
         <v>46.5</v>
       </c>
       <c r="AQ22" s="22"/>
       <c r="AR22" s="22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AS22" s="22">
         <v>67.5</v>
       </c>
       <c r="AT22" s="22"/>
       <c r="AU22" s="22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AV22" s="22">
         <v>29.8</v>
       </c>
       <c r="AW22" s="22"/>
       <c r="AX22" s="22" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AY22" s="22">
         <v>41.6</v>
       </c>
       <c r="AZ22" s="22"/>
       <c r="BA22" s="22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="BB22" s="23">
         <v>53.3</v>
@@ -2887,7 +2862,7 @@
         <v>20</v>
       </c>
       <c r="B23" s="22" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C23" s="22">
         <v>29.6</v>
@@ -2901,14 +2876,14 @@
       </c>
       <c r="G23" s="22"/>
       <c r="H23" s="22" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I23" s="23">
         <v>51</v>
       </c>
       <c r="J23" s="22"/>
       <c r="K23" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L23" s="23">
         <v>40.200000000000003</v>
@@ -2922,7 +2897,7 @@
       </c>
       <c r="P23" s="22"/>
       <c r="Q23" s="22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="R23" s="23">
         <v>49.6</v>
@@ -2957,7 +2932,7 @@
       </c>
       <c r="AE23" s="22"/>
       <c r="AF23" s="22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AG23" s="22">
         <v>32.4</v>
@@ -2971,21 +2946,21 @@
       </c>
       <c r="AK23" s="22"/>
       <c r="AL23" s="22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AM23" s="22">
         <v>46.4</v>
       </c>
       <c r="AN23" s="22"/>
       <c r="AO23" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AP23" s="22">
         <v>32.4</v>
       </c>
       <c r="AQ23" s="22"/>
       <c r="AR23" s="22" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AS23" s="22">
         <v>47.7</v>
@@ -3006,7 +2981,7 @@
       </c>
       <c r="AZ23" s="22"/>
       <c r="BA23" s="22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="BB23" s="22">
         <v>29.6</v>
@@ -3024,28 +2999,28 @@
         <v>21</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C24" s="23">
         <v>57.8</v>
       </c>
       <c r="D24" s="22"/>
       <c r="E24" s="21" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F24" s="22">
         <v>43.9</v>
       </c>
       <c r="G24" s="22"/>
       <c r="H24" s="21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I24" s="23">
         <v>40.799999999999997</v>
       </c>
       <c r="J24" s="22"/>
       <c r="K24" s="21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L24" s="22">
         <v>36.9</v>
@@ -3059,35 +3034,35 @@
       </c>
       <c r="P24" s="22"/>
       <c r="Q24" s="21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="R24" s="22">
         <v>57.6</v>
       </c>
       <c r="S24" s="22"/>
       <c r="T24" s="21" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="U24" s="22">
         <v>51.1</v>
       </c>
       <c r="V24" s="22"/>
       <c r="W24" s="21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="X24" s="22">
         <v>73.900000000000006</v>
       </c>
       <c r="Y24" s="22"/>
       <c r="Z24" s="21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AA24" s="22">
         <v>67.599999999999994</v>
       </c>
       <c r="AB24" s="22"/>
       <c r="AC24" s="21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AD24" s="22">
         <v>57.7</v>
@@ -3101,42 +3076,42 @@
       </c>
       <c r="AH24" s="22"/>
       <c r="AI24" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AJ24" s="22">
         <v>41.8</v>
       </c>
       <c r="AK24" s="22"/>
       <c r="AL24" s="21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="AM24" s="22">
         <v>63.8</v>
       </c>
       <c r="AN24" s="22"/>
       <c r="AO24" s="21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AP24" s="22">
         <v>42.6</v>
       </c>
       <c r="AQ24" s="22"/>
       <c r="AR24" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="AS24" s="22" t="s">
         <v>42</v>
-      </c>
-      <c r="AS24" s="22" t="s">
-        <v>43</v>
       </c>
       <c r="AT24" s="22"/>
       <c r="AU24" s="21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AV24" s="22">
         <v>60.3</v>
       </c>
       <c r="AW24" s="22"/>
       <c r="AX24" s="21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AY24" s="22">
         <v>58.2</v>
@@ -3175,14 +3150,14 @@
       </c>
       <c r="G25" s="22"/>
       <c r="H25" s="21" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I25" s="23">
         <v>39.200000000000003</v>
       </c>
       <c r="J25" s="22"/>
       <c r="K25" s="21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L25" s="22">
         <v>37.1</v>
@@ -3196,7 +3171,7 @@
       </c>
       <c r="P25" s="22"/>
       <c r="Q25" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="R25" s="22">
         <v>27.3</v>
@@ -3231,7 +3206,7 @@
       </c>
       <c r="AE25" s="22"/>
       <c r="AF25" s="21" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AG25" s="22">
         <v>29.3</v>
@@ -3298,31 +3273,31 @@
         <v>23</v>
       </c>
       <c r="B26" s="21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C26" s="23">
         <v>63.9</v>
       </c>
       <c r="D26" s="22"/>
       <c r="E26" s="21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F26" s="22">
         <v>63.8</v>
       </c>
       <c r="G26" s="22"/>
       <c r="H26" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="I26" s="23" t="s">
         <v>42</v>
-      </c>
-      <c r="I26" s="23" t="s">
-        <v>43</v>
       </c>
       <c r="J26" s="22"/>
       <c r="K26" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="L26" s="23" t="s">
         <v>42</v>
-      </c>
-      <c r="L26" s="23" t="s">
-        <v>43</v>
       </c>
       <c r="M26" s="22"/>
       <c r="N26" s="21">
@@ -3333,49 +3308,49 @@
       </c>
       <c r="P26" s="22"/>
       <c r="Q26" s="21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="R26" s="23">
         <v>63.8</v>
       </c>
       <c r="S26" s="22"/>
       <c r="T26" s="21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U26" s="23">
         <v>40.1</v>
       </c>
       <c r="V26" s="22"/>
       <c r="W26" s="21" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="X26" s="23">
         <v>46.3</v>
       </c>
       <c r="Y26" s="22"/>
       <c r="Z26" s="21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AA26" s="23">
         <v>67.599999999999994</v>
       </c>
       <c r="AB26" s="22"/>
       <c r="AC26" s="21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="AD26" s="23">
         <v>85.4</v>
       </c>
       <c r="AE26" s="22"/>
       <c r="AF26" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG26" s="23" t="s">
         <v>42</v>
-      </c>
-      <c r="AG26" s="23" t="s">
-        <v>43</v>
       </c>
       <c r="AH26" s="22"/>
       <c r="AI26" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AJ26" s="23">
         <v>37.700000000000003</v>
@@ -3389,35 +3364,35 @@
       </c>
       <c r="AN26" s="22"/>
       <c r="AO26" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="AP26" s="23" t="s">
         <v>42</v>
-      </c>
-      <c r="AP26" s="23" t="s">
-        <v>43</v>
       </c>
       <c r="AQ26" s="22"/>
       <c r="AR26" s="21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AS26" s="23">
         <v>29.5</v>
       </c>
       <c r="AT26" s="22"/>
       <c r="AU26" s="21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AV26" s="23">
         <v>63.7</v>
       </c>
       <c r="AW26" s="22"/>
       <c r="AX26" s="21" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AY26" s="23">
         <v>61.1</v>
       </c>
       <c r="AZ26" s="22"/>
       <c r="BA26" s="21" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="BB26" s="23">
         <v>85.3</v>
@@ -3435,28 +3410,28 @@
         <v>24</v>
       </c>
       <c r="B27" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" s="23" t="s">
         <v>42</v>
-      </c>
-      <c r="C27" s="23" t="s">
-        <v>43</v>
       </c>
       <c r="D27" s="22"/>
       <c r="E27" s="21" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F27" s="22">
         <v>49.5</v>
       </c>
       <c r="G27" s="22"/>
       <c r="H27" s="21" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I27" s="22">
         <v>85.3</v>
       </c>
       <c r="J27" s="22"/>
       <c r="K27" s="22" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L27" s="23">
         <v>60.6</v>
@@ -3470,59 +3445,59 @@
       </c>
       <c r="P27" s="22"/>
       <c r="Q27" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="R27" s="23" t="s">
         <v>42</v>
-      </c>
-      <c r="R27" s="23" t="s">
-        <v>43</v>
       </c>
       <c r="S27" s="22"/>
       <c r="T27" s="22" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="U27" s="23">
         <v>42.9</v>
       </c>
       <c r="V27" s="22"/>
       <c r="W27" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="X27" s="23" t="s">
         <v>42</v>
-      </c>
-      <c r="X27" s="23" t="s">
-        <v>43</v>
       </c>
       <c r="Y27" s="22"/>
       <c r="Z27" s="22" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AA27" s="23">
         <v>61.1</v>
       </c>
       <c r="AB27" s="22"/>
       <c r="AC27" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AD27" s="23">
         <v>63.6</v>
       </c>
       <c r="AE27" s="22"/>
       <c r="AF27" s="22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AG27" s="23">
         <v>58</v>
       </c>
       <c r="AH27" s="22"/>
       <c r="AI27" s="22" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AJ27" s="23">
         <v>57.7</v>
       </c>
       <c r="AK27" s="22"/>
       <c r="AL27" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="AM27" s="23" t="s">
         <v>42</v>
-      </c>
-      <c r="AM27" s="23" t="s">
-        <v>43</v>
       </c>
       <c r="AN27" s="22"/>
       <c r="AO27" s="22">
@@ -3533,28 +3508,28 @@
       </c>
       <c r="AQ27" s="22"/>
       <c r="AR27" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="AS27" s="23" t="s">
         <v>42</v>
-      </c>
-      <c r="AS27" s="23" t="s">
-        <v>43</v>
       </c>
       <c r="AT27" s="22"/>
       <c r="AU27" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="AV27" s="23" t="s">
         <v>42</v>
-      </c>
-      <c r="AV27" s="23" t="s">
-        <v>43</v>
       </c>
       <c r="AW27" s="22"/>
       <c r="AX27" s="22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AY27" s="23">
         <v>55.2</v>
       </c>
       <c r="AZ27" s="22"/>
       <c r="BA27" s="22" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="BB27" s="23">
         <v>55.4</v>
@@ -3569,750 +3544,690 @@
     </row>
     <row r="28" spans="1:57" ht="15.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="B28" s="21"/>
-      <c r="C28" s="23"/>
+        <v>29</v>
+      </c>
+      <c r="B28" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" s="23">
+        <v>67.599999999999994</v>
+      </c>
       <c r="D28" s="22"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="22"/>
+      <c r="E28" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="F28" s="22">
+        <v>64.099999999999994</v>
+      </c>
       <c r="G28" s="22"/>
-      <c r="H28" s="21"/>
-      <c r="I28" s="22"/>
+      <c r="H28" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="I28" s="22">
+        <v>86.6</v>
+      </c>
       <c r="J28" s="22"/>
-      <c r="K28" s="22"/>
-      <c r="L28" s="23"/>
+      <c r="K28" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="L28" s="23">
+        <v>72.3</v>
+      </c>
       <c r="M28" s="22"/>
-      <c r="N28" s="22"/>
-      <c r="O28" s="23"/>
+      <c r="N28" s="22">
+        <v>548</v>
+      </c>
+      <c r="O28" s="23">
+        <v>15.9</v>
+      </c>
       <c r="P28" s="22"/>
-      <c r="Q28" s="22"/>
-      <c r="R28" s="23"/>
+      <c r="Q28" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="R28" s="23">
+        <v>51</v>
+      </c>
       <c r="S28" s="22"/>
-      <c r="T28" s="22"/>
-      <c r="U28" s="23"/>
+      <c r="T28" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="U28" s="23">
+        <v>46.4</v>
+      </c>
       <c r="V28" s="22"/>
-      <c r="W28" s="22"/>
-      <c r="X28" s="23"/>
+      <c r="W28" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="X28" s="23">
+        <v>39.799999999999997</v>
+      </c>
       <c r="Y28" s="22"/>
-      <c r="Z28" s="22"/>
-      <c r="AA28" s="23"/>
+      <c r="Z28" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="AA28" s="23">
+        <v>55.3</v>
+      </c>
       <c r="AB28" s="22"/>
-      <c r="AC28" s="22"/>
-      <c r="AD28" s="23"/>
+      <c r="AC28" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="AD28" s="23">
+        <v>58</v>
+      </c>
       <c r="AE28" s="22"/>
-      <c r="AF28" s="22"/>
-      <c r="AG28" s="23"/>
+      <c r="AF28" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="AG28" s="23">
+        <v>78.400000000000006</v>
+      </c>
       <c r="AH28" s="22"/>
-      <c r="AI28" s="22"/>
-      <c r="AJ28" s="23"/>
+      <c r="AI28" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="AJ28" s="23">
+        <v>30.6</v>
+      </c>
       <c r="AK28" s="22"/>
-      <c r="AL28" s="22"/>
-      <c r="AM28" s="23"/>
+      <c r="AL28" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="AM28" s="23">
+        <v>32</v>
+      </c>
       <c r="AN28" s="22"/>
-      <c r="AO28" s="22"/>
-      <c r="AP28" s="23"/>
+      <c r="AO28" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="AP28" s="23">
+        <v>85.3</v>
+      </c>
       <c r="AQ28" s="22"/>
-      <c r="AR28" s="22"/>
-      <c r="AS28" s="23"/>
+      <c r="AR28" s="22">
+        <v>439</v>
+      </c>
+      <c r="AS28" s="23">
+        <v>17.100000000000001</v>
+      </c>
       <c r="AT28" s="22"/>
-      <c r="AU28" s="22"/>
-      <c r="AV28" s="23"/>
+      <c r="AU28" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="AV28" s="23">
+        <v>49.4</v>
+      </c>
       <c r="AW28" s="22"/>
-      <c r="AX28" s="22"/>
-      <c r="AY28" s="23"/>
+      <c r="AX28" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="AY28" s="23">
+        <v>58</v>
+      </c>
       <c r="AZ28" s="22"/>
-      <c r="BA28" s="22"/>
-      <c r="BB28" s="23"/>
+      <c r="BA28" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="BB28" s="23">
+        <v>63.9</v>
+      </c>
       <c r="BC28" s="23"/>
-      <c r="BD28" s="22"/>
-      <c r="BE28" s="23"/>
+      <c r="BD28" s="22">
+        <v>1801</v>
+      </c>
+      <c r="BE28" s="23">
+        <v>8.6</v>
+      </c>
     </row>
     <row r="29" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B29" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="C29" s="23">
-        <v>67.599999999999994</v>
+      <c r="A29" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="C29" s="22">
+        <v>29.6</v>
       </c>
       <c r="D29" s="22"/>
-      <c r="E29" s="21" t="s">
-        <v>125</v>
+      <c r="E29" s="22" t="s">
+        <v>72</v>
       </c>
       <c r="F29" s="22">
-        <v>64.099999999999994</v>
+        <v>30.2</v>
       </c>
       <c r="G29" s="22"/>
-      <c r="H29" s="21" t="s">
-        <v>120</v>
+      <c r="H29" s="22" t="s">
+        <v>75</v>
       </c>
       <c r="I29" s="22">
-        <v>86.6</v>
+        <v>53.1</v>
       </c>
       <c r="J29" s="22"/>
       <c r="K29" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="L29" s="23">
-        <v>72.3</v>
+        <v>129</v>
+      </c>
+      <c r="L29" s="22">
+        <v>51.2</v>
       </c>
       <c r="M29" s="22"/>
       <c r="N29" s="22">
-        <v>548</v>
-      </c>
-      <c r="O29" s="23">
-        <v>15.9</v>
+        <v>903</v>
+      </c>
+      <c r="O29" s="22">
+        <v>12.5</v>
       </c>
       <c r="P29" s="22"/>
       <c r="Q29" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="R29" s="23">
         <v>51</v>
       </c>
+      <c r="R29" s="22">
+        <v>40.799999999999997</v>
+      </c>
       <c r="S29" s="22"/>
-      <c r="T29" s="22" t="s">
-        <v>107</v>
-      </c>
-      <c r="U29" s="23">
-        <v>46.4</v>
+      <c r="T29" s="22">
+        <v>222</v>
+      </c>
+      <c r="U29" s="22">
+        <v>24.6</v>
       </c>
       <c r="V29" s="22"/>
-      <c r="W29" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="X29" s="23">
-        <v>39.799999999999997</v>
+      <c r="W29" s="22">
+        <v>294</v>
+      </c>
+      <c r="X29" s="22">
+        <v>21.5</v>
       </c>
       <c r="Y29" s="22"/>
-      <c r="Z29" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="AA29" s="23">
-        <v>55.3</v>
+      <c r="Z29" s="22">
+        <v>190</v>
+      </c>
+      <c r="AA29" s="22">
+        <v>26.8</v>
       </c>
       <c r="AB29" s="22"/>
       <c r="AC29" s="22" t="s">
-        <v>126</v>
+        <v>96</v>
       </c>
       <c r="AD29" s="23">
-        <v>58</v>
+        <v>46.4</v>
       </c>
       <c r="AE29" s="22"/>
       <c r="AF29" s="22" t="s">
-        <v>127</v>
-      </c>
-      <c r="AG29" s="23">
-        <v>78.400000000000006</v>
+        <v>103</v>
+      </c>
+      <c r="AG29" s="22">
+        <v>51.1</v>
       </c>
       <c r="AH29" s="22"/>
-      <c r="AI29" s="22" t="s">
-        <v>128</v>
-      </c>
-      <c r="AJ29" s="23">
-        <v>30.6</v>
+      <c r="AI29" s="22">
+        <v>494</v>
+      </c>
+      <c r="AJ29" s="22">
+        <v>16.600000000000001</v>
       </c>
       <c r="AK29" s="22"/>
       <c r="AL29" s="22" t="s">
-        <v>106</v>
-      </c>
-      <c r="AM29" s="23">
-        <v>32</v>
+        <v>62</v>
+      </c>
+      <c r="AM29" s="22">
+        <v>46.4</v>
       </c>
       <c r="AN29" s="22"/>
       <c r="AO29" s="22" t="s">
-        <v>122</v>
-      </c>
-      <c r="AP29" s="23">
-        <v>85.3</v>
+        <v>48</v>
+      </c>
+      <c r="AP29" s="22">
+        <v>62.8</v>
       </c>
       <c r="AQ29" s="22"/>
-      <c r="AR29" s="22">
-        <v>439</v>
-      </c>
-      <c r="AS29" s="23">
-        <v>17.100000000000001</v>
+      <c r="AR29" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="AS29" s="22">
+        <v>51.1</v>
       </c>
       <c r="AT29" s="22"/>
-      <c r="AU29" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="AV29" s="23">
-        <v>49.4</v>
+      <c r="AU29" s="22">
+        <v>892</v>
+      </c>
+      <c r="AV29" s="22">
+        <v>12.2</v>
       </c>
       <c r="AW29" s="22"/>
       <c r="AX29" s="22" t="s">
-        <v>65</v>
-      </c>
-      <c r="AY29" s="23">
-        <v>58</v>
+        <v>51</v>
+      </c>
+      <c r="AY29" s="22">
+        <v>42.3</v>
       </c>
       <c r="AZ29" s="22"/>
       <c r="BA29" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="BB29" s="23">
-        <v>63.9</v>
-      </c>
-      <c r="BC29" s="23"/>
-      <c r="BD29" s="22">
-        <v>1801</v>
-      </c>
-      <c r="BE29" s="23">
-        <v>8.6</v>
+        <v>69</v>
+      </c>
+      <c r="BB29" s="22">
+        <v>43.8</v>
+      </c>
+      <c r="BC29" s="22"/>
+      <c r="BD29" s="21">
+        <v>3869</v>
+      </c>
+      <c r="BE29" s="22">
+        <v>5.9</v>
       </c>
     </row>
     <row r="30" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B30" s="22" t="s">
-        <v>129</v>
+      <c r="A30" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" s="21" t="s">
+        <v>51</v>
       </c>
       <c r="C30" s="22">
-        <v>29.6</v>
+        <v>39.799999999999997</v>
       </c>
       <c r="D30" s="22"/>
-      <c r="E30" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="F30" s="22">
-        <v>30.2</v>
+      <c r="E30" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="F30" s="23">
+        <v>45</v>
       </c>
       <c r="G30" s="22"/>
-      <c r="H30" s="22" t="s">
-        <v>76</v>
+      <c r="H30" s="21" t="s">
+        <v>55</v>
       </c>
       <c r="I30" s="22">
-        <v>53.1</v>
+        <v>85.8</v>
       </c>
       <c r="J30" s="22"/>
-      <c r="K30" s="22" t="s">
+      <c r="K30" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="L30" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="M30" s="22"/>
+      <c r="N30" s="21">
+        <v>338</v>
+      </c>
+      <c r="O30" s="22">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="P30" s="22"/>
+      <c r="Q30" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="R30" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="S30" s="22"/>
+      <c r="T30" s="21" t="s">
         <v>130</v>
       </c>
-      <c r="L30" s="22">
-        <v>51.2</v>
-      </c>
-      <c r="M30" s="22"/>
-      <c r="N30" s="22">
-        <v>903</v>
-      </c>
-      <c r="O30" s="22">
-        <v>12.5</v>
-      </c>
-      <c r="P30" s="22"/>
-      <c r="Q30" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="R30" s="22">
-        <v>40.799999999999997</v>
-      </c>
-      <c r="S30" s="22"/>
-      <c r="T30" s="22">
-        <v>222</v>
-      </c>
       <c r="U30" s="22">
-        <v>24.6</v>
+        <v>33.299999999999997</v>
       </c>
       <c r="V30" s="22"/>
-      <c r="W30" s="22">
-        <v>294</v>
+      <c r="W30" s="21" t="s">
+        <v>125</v>
       </c>
       <c r="X30" s="22">
-        <v>21.5</v>
+        <v>57.7</v>
       </c>
       <c r="Y30" s="22"/>
-      <c r="Z30" s="22">
-        <v>190</v>
-      </c>
-      <c r="AA30" s="22">
-        <v>26.8</v>
+      <c r="Z30" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA30" s="23">
+        <v>37.799999999999997</v>
       </c>
       <c r="AB30" s="22"/>
-      <c r="AC30" s="22" t="s">
-        <v>97</v>
-      </c>
-      <c r="AD30" s="23">
-        <v>46.4</v>
+      <c r="AC30" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="AD30" s="22">
+        <v>60.3</v>
       </c>
       <c r="AE30" s="22"/>
-      <c r="AF30" s="22" t="s">
-        <v>104</v>
-      </c>
-      <c r="AG30" s="22">
-        <v>51.1</v>
+      <c r="AF30" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="AG30" s="23">
+        <v>60.2</v>
       </c>
       <c r="AH30" s="22"/>
-      <c r="AI30" s="22">
-        <v>494</v>
+      <c r="AI30" s="21" t="s">
+        <v>99</v>
       </c>
       <c r="AJ30" s="22">
-        <v>16.600000000000001</v>
+        <v>51.5</v>
       </c>
       <c r="AK30" s="22"/>
-      <c r="AL30" s="22" t="s">
-        <v>63</v>
+      <c r="AL30" s="21" t="s">
+        <v>55</v>
       </c>
       <c r="AM30" s="22">
-        <v>46.4</v>
+        <v>85.4</v>
       </c>
       <c r="AN30" s="22"/>
-      <c r="AO30" s="22" t="s">
-        <v>49</v>
+      <c r="AO30" s="21" t="s">
+        <v>59</v>
       </c>
       <c r="AP30" s="22">
-        <v>62.8</v>
+        <v>60.8</v>
       </c>
       <c r="AQ30" s="22"/>
-      <c r="AR30" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="AS30" s="22">
-        <v>51.1</v>
+      <c r="AR30" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="AS30" s="22" t="s">
+        <v>42</v>
       </c>
       <c r="AT30" s="22"/>
-      <c r="AU30" s="22">
-        <v>892</v>
+      <c r="AU30" s="21" t="s">
+        <v>51</v>
       </c>
       <c r="AV30" s="22">
-        <v>12.2</v>
+        <v>39.799999999999997</v>
       </c>
       <c r="AW30" s="22"/>
-      <c r="AX30" s="22" t="s">
-        <v>52</v>
+      <c r="AX30" s="21">
+        <v>369</v>
       </c>
       <c r="AY30" s="22">
-        <v>42.3</v>
+        <v>18.8</v>
       </c>
       <c r="AZ30" s="22"/>
-      <c r="BA30" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="BB30" s="22">
-        <v>43.8</v>
+      <c r="BA30" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="BB30" s="23">
+        <v>86</v>
       </c>
       <c r="BC30" s="22"/>
       <c r="BD30" s="21">
-        <v>3869</v>
+        <v>1424</v>
       </c>
       <c r="BE30" s="22">
-        <v>5.9</v>
+        <v>9.6</v>
       </c>
     </row>
     <row r="31" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>32</v>
+      <c r="A31" s="25" t="s">
+        <v>30</v>
       </c>
       <c r="B31" s="21" t="s">
-        <v>52</v>
+        <v>123</v>
       </c>
       <c r="C31" s="22">
-        <v>39.799999999999997</v>
+        <v>55.5</v>
       </c>
       <c r="D31" s="22"/>
       <c r="E31" s="21" t="s">
-        <v>88</v>
+        <v>131</v>
       </c>
       <c r="F31" s="23">
-        <v>45</v>
+        <v>32.299999999999997</v>
       </c>
       <c r="G31" s="22"/>
       <c r="H31" s="21" t="s">
-        <v>56</v>
+        <v>132</v>
       </c>
       <c r="I31" s="22">
-        <v>85.8</v>
+        <v>30.7</v>
       </c>
       <c r="J31" s="22"/>
       <c r="K31" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="L31" s="22" t="s">
-        <v>43</v>
+        <v>133</v>
+      </c>
+      <c r="L31" s="22">
+        <v>29.2</v>
       </c>
       <c r="M31" s="22"/>
       <c r="N31" s="21">
-        <v>338</v>
+        <v>1495</v>
       </c>
       <c r="O31" s="22">
-        <v>20.399999999999999</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="P31" s="22"/>
       <c r="Q31" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="R31" s="22" t="s">
-        <v>43</v>
+        <v>62</v>
+      </c>
+      <c r="R31" s="22">
+        <v>47.9</v>
       </c>
       <c r="S31" s="22"/>
       <c r="T31" s="21" t="s">
-        <v>131</v>
+        <v>81</v>
       </c>
       <c r="U31" s="22">
-        <v>33.299999999999997</v>
+        <v>29.1</v>
       </c>
       <c r="V31" s="22"/>
       <c r="W31" s="21" t="s">
-        <v>126</v>
+        <v>50</v>
       </c>
       <c r="X31" s="22">
-        <v>57.7</v>
+        <v>34.1</v>
       </c>
       <c r="Y31" s="22"/>
       <c r="Z31" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="AA31" s="23">
-        <v>37.799999999999997</v>
+        <v>82</v>
+      </c>
+      <c r="AA31" s="22">
+        <v>37.5</v>
       </c>
       <c r="AB31" s="22"/>
       <c r="AC31" s="21" t="s">
-        <v>60</v>
+        <v>123</v>
       </c>
       <c r="AD31" s="22">
-        <v>60.3</v>
+        <v>55.1</v>
       </c>
       <c r="AE31" s="22"/>
-      <c r="AF31" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="AG31" s="23">
-        <v>60.2</v>
+      <c r="AF31" s="21">
+        <v>222</v>
+      </c>
+      <c r="AG31" s="22">
+        <v>24.5</v>
       </c>
       <c r="AH31" s="22"/>
-      <c r="AI31" s="21" t="s">
-        <v>100</v>
+      <c r="AI31" s="21">
+        <v>190</v>
       </c>
       <c r="AJ31" s="22">
-        <v>51.5</v>
+        <v>26.6</v>
       </c>
       <c r="AK31" s="22"/>
       <c r="AL31" s="21" t="s">
-        <v>56</v>
+        <v>104</v>
       </c>
       <c r="AM31" s="22">
-        <v>85.4</v>
+        <v>47.7</v>
       </c>
       <c r="AN31" s="22"/>
       <c r="AO31" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="AP31" s="22">
-        <v>60.8</v>
+        <v>134</v>
+      </c>
+      <c r="AP31" s="23">
+        <v>35.700000000000003</v>
       </c>
       <c r="AQ31" s="22"/>
       <c r="AR31" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="AS31" s="22" t="s">
-        <v>43</v>
+        <v>123</v>
+      </c>
+      <c r="AS31" s="22">
+        <v>55.2</v>
       </c>
       <c r="AT31" s="22"/>
       <c r="AU31" s="21" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AV31" s="22">
-        <v>39.799999999999997</v>
+        <v>39.1</v>
       </c>
       <c r="AW31" s="22"/>
-      <c r="AX31" s="21">
-        <v>369</v>
+      <c r="AX31" s="21" t="s">
+        <v>135</v>
       </c>
       <c r="AY31" s="22">
-        <v>18.8</v>
+        <v>45.1</v>
       </c>
       <c r="AZ31" s="22"/>
-      <c r="BA31" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="BB31" s="23">
-        <v>86</v>
+      <c r="BA31" s="21">
+        <v>1796</v>
+      </c>
+      <c r="BB31" s="22">
+        <v>8.5</v>
       </c>
       <c r="BC31" s="22"/>
       <c r="BD31" s="21">
-        <v>1424</v>
+        <v>5009</v>
       </c>
       <c r="BE31" s="22">
-        <v>9.6</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="32" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B32" s="21" t="s">
-        <v>124</v>
-      </c>
-      <c r="C32" s="22">
-        <v>55.5</v>
-      </c>
-      <c r="D32" s="22"/>
-      <c r="E32" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="F32" s="23">
-        <v>32.299999999999997</v>
-      </c>
-      <c r="G32" s="22"/>
-      <c r="H32" s="21" t="s">
-        <v>133</v>
-      </c>
-      <c r="I32" s="22">
-        <v>30.7</v>
-      </c>
-      <c r="J32" s="22"/>
-      <c r="K32" s="21" t="s">
-        <v>134</v>
-      </c>
-      <c r="L32" s="22">
-        <v>29.2</v>
-      </c>
-      <c r="M32" s="22"/>
-      <c r="N32" s="21">
-        <v>1495</v>
-      </c>
-      <c r="O32" s="22">
-        <v>9.8000000000000007</v>
-      </c>
-      <c r="P32" s="22"/>
-      <c r="Q32" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="R32" s="22">
-        <v>47.9</v>
-      </c>
-      <c r="S32" s="22"/>
-      <c r="T32" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="U32" s="22">
-        <v>29.1</v>
-      </c>
-      <c r="V32" s="22"/>
-      <c r="W32" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="X32" s="22">
-        <v>34.1</v>
-      </c>
-      <c r="Y32" s="22"/>
-      <c r="Z32" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="AA32" s="22">
-        <v>37.5</v>
-      </c>
-      <c r="AB32" s="22"/>
-      <c r="AC32" s="21" t="s">
-        <v>124</v>
-      </c>
-      <c r="AD32" s="22">
-        <v>55.1</v>
-      </c>
-      <c r="AE32" s="22"/>
-      <c r="AF32" s="21">
-        <v>222</v>
-      </c>
-      <c r="AG32" s="22">
-        <v>24.5</v>
-      </c>
-      <c r="AH32" s="22"/>
-      <c r="AI32" s="21">
-        <v>190</v>
-      </c>
-      <c r="AJ32" s="22">
-        <v>26.6</v>
-      </c>
-      <c r="AK32" s="22"/>
-      <c r="AL32" s="21" t="s">
-        <v>105</v>
-      </c>
-      <c r="AM32" s="22">
-        <v>47.7</v>
-      </c>
-      <c r="AN32" s="22"/>
-      <c r="AO32" s="21" t="s">
-        <v>135</v>
-      </c>
-      <c r="AP32" s="23">
-        <v>35.700000000000003</v>
-      </c>
-      <c r="AQ32" s="22"/>
-      <c r="AR32" s="21" t="s">
-        <v>124</v>
-      </c>
-      <c r="AS32" s="22">
-        <v>55.2</v>
-      </c>
-      <c r="AT32" s="22"/>
-      <c r="AU32" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="AV32" s="22">
-        <v>39.1</v>
-      </c>
-      <c r="AW32" s="22"/>
-      <c r="AX32" s="21" t="s">
-        <v>136</v>
-      </c>
-      <c r="AY32" s="22">
-        <v>45.1</v>
-      </c>
-      <c r="AZ32" s="22"/>
-      <c r="BA32" s="21">
-        <v>1796</v>
-      </c>
-      <c r="BB32" s="22">
-        <v>8.5</v>
-      </c>
-      <c r="BC32" s="22"/>
-      <c r="BD32" s="21">
-        <v>5009</v>
-      </c>
-      <c r="BE32" s="22">
+      <c r="A32" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" s="14">
+        <v>3893</v>
+      </c>
+      <c r="C32" s="8">
+        <v>5.7</v>
+      </c>
+      <c r="D32" s="8"/>
+      <c r="E32" s="14">
+        <v>8210</v>
+      </c>
+      <c r="F32" s="15">
+        <v>4</v>
+      </c>
+      <c r="G32" s="8"/>
+      <c r="H32" s="14">
+        <v>3592</v>
+      </c>
+      <c r="I32" s="15">
+        <v>6</v>
+      </c>
+      <c r="J32" s="8"/>
+      <c r="K32" s="14">
+        <v>3194</v>
+      </c>
+      <c r="L32" s="8">
+        <v>6.4</v>
+      </c>
+      <c r="M32" s="8"/>
+      <c r="N32" s="14">
+        <v>69269</v>
+      </c>
+      <c r="O32" s="8">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="P32" s="8"/>
+      <c r="Q32" s="14">
+        <v>3549</v>
+      </c>
+      <c r="R32" s="15">
+        <v>6</v>
+      </c>
+      <c r="S32" s="8"/>
+      <c r="T32" s="14">
+        <v>11737</v>
+      </c>
+      <c r="U32" s="8">
+        <v>3.3</v>
+      </c>
+      <c r="V32" s="8"/>
+      <c r="W32" s="14">
+        <v>7258</v>
+      </c>
+      <c r="X32" s="8">
+        <v>4.2</v>
+      </c>
+      <c r="Y32" s="8"/>
+      <c r="Z32" s="14">
+        <v>6419</v>
+      </c>
+      <c r="AA32" s="8">
+        <v>4.5</v>
+      </c>
+      <c r="AB32" s="8"/>
+      <c r="AC32" s="14">
+        <v>4122</v>
+      </c>
+      <c r="AD32" s="8">
+        <v>5.6</v>
+      </c>
+      <c r="AE32" s="8"/>
+      <c r="AF32" s="14">
+        <v>4727</v>
+      </c>
+      <c r="AG32" s="8">
         <v>5.2</v>
       </c>
+      <c r="AH32" s="8"/>
+      <c r="AI32" s="14">
+        <v>11219</v>
+      </c>
+      <c r="AJ32" s="8">
+        <v>3.4</v>
+      </c>
+      <c r="AK32" s="8"/>
+      <c r="AL32" s="14">
+        <v>3750</v>
+      </c>
+      <c r="AM32" s="8">
+        <v>5.9</v>
+      </c>
+      <c r="AN32" s="8"/>
+      <c r="AO32" s="14">
+        <v>4228</v>
+      </c>
+      <c r="AP32" s="8">
+        <v>5.5</v>
+      </c>
+      <c r="AQ32" s="8"/>
+      <c r="AR32" s="14">
+        <v>3384</v>
+      </c>
+      <c r="AS32" s="15">
+        <v>6.1</v>
+      </c>
+      <c r="AT32" s="8"/>
+      <c r="AU32" s="14">
+        <v>5997</v>
+      </c>
+      <c r="AV32" s="8">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="AW32" s="8"/>
+      <c r="AX32" s="14">
+        <v>4522</v>
+      </c>
+      <c r="AY32" s="8">
+        <v>5.3</v>
+      </c>
+      <c r="AZ32" s="8"/>
+      <c r="BA32" s="14">
+        <v>9810</v>
+      </c>
+      <c r="BB32" s="8">
+        <v>3.6</v>
+      </c>
+      <c r="BC32" s="8"/>
+      <c r="BD32" s="14">
+        <v>168881</v>
+      </c>
+      <c r="BE32" s="8">
+        <v>0.7</v>
+      </c>
     </row>
-    <row r="33" spans="1:57" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B33" s="14">
-        <v>3893</v>
-      </c>
-      <c r="C33" s="8">
-        <v>5.7</v>
-      </c>
-      <c r="D33" s="8"/>
-      <c r="E33" s="14">
-        <v>8210</v>
-      </c>
-      <c r="F33" s="15">
-        <v>4</v>
-      </c>
-      <c r="G33" s="8"/>
-      <c r="H33" s="14">
-        <v>3592</v>
-      </c>
-      <c r="I33" s="15">
-        <v>6</v>
-      </c>
-      <c r="J33" s="8"/>
-      <c r="K33" s="14">
-        <v>3194</v>
-      </c>
-      <c r="L33" s="8">
-        <v>6.4</v>
-      </c>
-      <c r="M33" s="8"/>
-      <c r="N33" s="14">
-        <v>69269</v>
-      </c>
-      <c r="O33" s="8">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="P33" s="8"/>
-      <c r="Q33" s="14">
-        <v>3549</v>
-      </c>
-      <c r="R33" s="15">
-        <v>6</v>
-      </c>
-      <c r="S33" s="8"/>
-      <c r="T33" s="14">
-        <v>11737</v>
-      </c>
-      <c r="U33" s="8">
-        <v>3.3</v>
-      </c>
-      <c r="V33" s="8"/>
-      <c r="W33" s="14">
-        <v>7258</v>
-      </c>
-      <c r="X33" s="8">
-        <v>4.2</v>
-      </c>
-      <c r="Y33" s="8"/>
-      <c r="Z33" s="14">
-        <v>6419</v>
-      </c>
-      <c r="AA33" s="8">
-        <v>4.5</v>
-      </c>
-      <c r="AB33" s="8"/>
-      <c r="AC33" s="14">
-        <v>4122</v>
-      </c>
-      <c r="AD33" s="8">
-        <v>5.6</v>
-      </c>
-      <c r="AE33" s="8"/>
-      <c r="AF33" s="14">
-        <v>4727</v>
-      </c>
-      <c r="AG33" s="8">
-        <v>5.2</v>
-      </c>
-      <c r="AH33" s="8"/>
-      <c r="AI33" s="14">
-        <v>11219</v>
-      </c>
-      <c r="AJ33" s="8">
-        <v>3.4</v>
-      </c>
-      <c r="AK33" s="8"/>
-      <c r="AL33" s="14">
-        <v>3750</v>
-      </c>
-      <c r="AM33" s="8">
-        <v>5.9</v>
-      </c>
-      <c r="AN33" s="8"/>
-      <c r="AO33" s="14">
-        <v>4228</v>
-      </c>
-      <c r="AP33" s="8">
-        <v>5.5</v>
-      </c>
-      <c r="AQ33" s="8"/>
-      <c r="AR33" s="14">
-        <v>3384</v>
-      </c>
-      <c r="AS33" s="15">
-        <v>6.1</v>
-      </c>
-      <c r="AT33" s="8"/>
-      <c r="AU33" s="14">
-        <v>5997</v>
-      </c>
-      <c r="AV33" s="8">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="AW33" s="8"/>
-      <c r="AX33" s="14">
-        <v>4522</v>
-      </c>
-      <c r="AY33" s="8">
-        <v>5.3</v>
-      </c>
-      <c r="AZ33" s="8"/>
-      <c r="BA33" s="14">
-        <v>9810</v>
-      </c>
-      <c r="BB33" s="8">
-        <v>3.6</v>
-      </c>
-      <c r="BC33" s="8"/>
-      <c r="BD33" s="14">
-        <v>168881</v>
-      </c>
-      <c r="BE33" s="8">
-        <v>0.7</v>
-      </c>
-    </row>
+    <row r="33" spans="1:57" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="34" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
       <c r="B34" s="14"/>
@@ -4475,7 +4390,7 @@
       <c r="BA47"/>
       <c r="BD47"/>
       <c r="BE47" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="48" spans="1:57" ht="3.9" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>